<commit_message>
Not analyzing last frame
</commit_message>
<xml_diff>
--- a/DataIndex.xlsx
+++ b/DataIndex.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel\AppData\Local\Temp\scp22898\afs\crc.nd.edu\group\Zartman\Pavel\Project3Episcale\GrowthStudy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel\AppData\Local\Temp\scp47777\afs\crc.nd.edu\group\Zartman\Pavel\Project3Episcale\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="77">
   <si>
     <t>Growth_0.1_MR_1</t>
   </si>
@@ -243,6 +243,18 @@
   </si>
   <si>
     <t>Growth_0.2_noMR_7</t>
+  </si>
+  <si>
+    <t>g_min</t>
+  </si>
+  <si>
+    <t>g_max</t>
+  </si>
+  <si>
+    <t>Growth_0.3_MR_1</t>
+  </si>
+  <si>
+    <t>Growth_0.3_noMR_1</t>
   </si>
 </sst>
 </file>
@@ -637,11 +649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73:C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,9 +661,11 @@
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -664,8 +678,14 @@
       <c r="D1" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -678,8 +698,14 @@
       <c r="D2" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -692,8 +718,14 @@
       <c r="D3" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -706,8 +738,14 @@
       <c r="D4" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -720,8 +758,14 @@
       <c r="D5" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -734,8 +778,14 @@
       <c r="D6" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -748,8 +798,14 @@
       <c r="D7" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -762,8 +818,14 @@
       <c r="D8" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -776,8 +838,14 @@
       <c r="D9" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -790,8 +858,14 @@
       <c r="D10" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -804,8 +878,14 @@
       <c r="D11" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -818,8 +898,14 @@
       <c r="D12" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -832,8 +918,14 @@
       <c r="D13" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -846,8 +938,14 @@
       <c r="D14" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -860,8 +958,14 @@
       <c r="D15" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -874,8 +978,14 @@
       <c r="D16" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -888,8 +998,14 @@
       <c r="D17" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -902,8 +1018,14 @@
       <c r="D18" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -916,8 +1038,14 @@
       <c r="D19" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -930,8 +1058,14 @@
       <c r="D20" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -944,8 +1078,14 @@
       <c r="D21" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -958,8 +1098,14 @@
       <c r="D22" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -972,8 +1118,14 @@
       <c r="D23" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -986,8 +1138,14 @@
       <c r="D24" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1000,8 +1158,14 @@
       <c r="D25" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1014,8 +1178,14 @@
       <c r="D26" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1028,8 +1198,14 @@
       <c r="D27" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1042,8 +1218,14 @@
       <c r="D28" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1056,8 +1238,14 @@
       <c r="D29" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="1">
+        <v>0.15</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1070,8 +1258,14 @@
       <c r="D30" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1084,8 +1278,14 @@
       <c r="D31" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1098,8 +1298,14 @@
       <c r="D32" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1112,8 +1318,14 @@
       <c r="D33" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1126,8 +1338,14 @@
       <c r="D34" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F34" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1140,8 +1358,14 @@
       <c r="D35" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1154,8 +1378,14 @@
       <c r="D36" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1168,8 +1398,14 @@
       <c r="D37" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1182,8 +1418,14 @@
       <c r="D38" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1196,8 +1438,14 @@
       <c r="D39" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1210,8 +1458,14 @@
       <c r="D40" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F40" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -1224,8 +1478,14 @@
       <c r="D41" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -1238,8 +1498,14 @@
       <c r="D42" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F42" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -1252,8 +1518,14 @@
       <c r="D43" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F43" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1266,8 +1538,14 @@
       <c r="D44" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -1280,8 +1558,14 @@
       <c r="D45" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -1294,8 +1578,14 @@
       <c r="D46" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F46" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -1308,8 +1598,14 @@
       <c r="D47" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F47" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>36</v>
       </c>
@@ -1322,8 +1618,14 @@
       <c r="D48" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F48" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -1336,8 +1638,14 @@
       <c r="D49" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="F49" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>36</v>
       </c>
@@ -1350,8 +1658,14 @@
       <c r="D50" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F50" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -1364,8 +1678,14 @@
       <c r="D51" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>36</v>
       </c>
@@ -1378,8 +1698,14 @@
       <c r="D52" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -1392,8 +1718,14 @@
       <c r="D53" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F53" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>36</v>
       </c>
@@ -1406,8 +1738,14 @@
       <c r="D54" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F54" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -1420,8 +1758,14 @@
       <c r="D55" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F55" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -1434,8 +1778,14 @@
       <c r="D56" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -1448,8 +1798,14 @@
       <c r="D57" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F57" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -1462,8 +1818,14 @@
       <c r="D58" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F58" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>36</v>
       </c>
@@ -1476,8 +1838,14 @@
       <c r="D59" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="F59" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>36</v>
       </c>
@@ -1490,8 +1858,14 @@
       <c r="D60" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F60" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -1504,8 +1878,14 @@
       <c r="D61" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F61" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>36</v>
       </c>
@@ -1518,8 +1898,14 @@
       <c r="D62" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F62" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>36</v>
       </c>
@@ -1532,8 +1918,14 @@
       <c r="D63" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F63" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>36</v>
       </c>
@@ -1546,8 +1938,14 @@
       <c r="D64" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F64" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>36</v>
       </c>
@@ -1560,8 +1958,14 @@
       <c r="D65" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F65" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -1574,8 +1978,14 @@
       <c r="D66" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F66" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>36</v>
       </c>
@@ -1588,8 +1998,14 @@
       <c r="D67" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F67" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>36</v>
       </c>
@@ -1602,8 +2018,14 @@
       <c r="D68" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F68" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>36</v>
       </c>
@@ -1615,6 +2037,52 @@
       </c>
       <c r="D69" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="E69" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F69" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D70" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E70" s="1">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B71" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D71" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0.22499999999999998</v>
+      </c>
+      <c r="F71" s="1">
+        <v>0.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made scripts for handling simulation output, and processed data
</commit_message>
<xml_diff>
--- a/DataIndex.xlsx
+++ b/DataIndex.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel\AppData\Local\Temp\scp47777\afs\crc.nd.edu\group\Zartman\Pavel\Project3Episcale\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel\AppData\Local\Temp\scp00500\afs\crc.nd.edu\group\Zartman\Pavel\Project3Episcale\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,33 +32,18 @@
     <t>Label</t>
   </si>
   <si>
-    <t>Growth_0.1_noMR_1</t>
-  </si>
-  <si>
-    <t>Growth_0.2_noMR_1</t>
-  </si>
-  <si>
     <t>Growth_0.2_MR_1</t>
   </si>
   <si>
     <t>Growth_0.8_MR_1</t>
   </si>
   <si>
-    <t>Growth_0.8_noMR_1</t>
-  </si>
-  <si>
-    <t>Growth_1.6_noMR_1</t>
-  </si>
-  <si>
     <t>Growth_1.6_MR_1</t>
   </si>
   <si>
     <t>Growth_3.2_MR_1</t>
   </si>
   <si>
-    <t>Growth_3.2_noMR_1</t>
-  </si>
-  <si>
     <t>g_ave</t>
   </si>
   <si>
@@ -68,69 +53,36 @@
     <t>Growth_0.4_MR_1</t>
   </si>
   <si>
-    <t>Growth_0.4_noMR_1</t>
-  </si>
-  <si>
     <t>Growth_0.1_MR_2</t>
   </si>
   <si>
-    <t>Growth_0.1_noMR_2</t>
-  </si>
-  <si>
     <t>Growth_0.2_MR_2</t>
   </si>
   <si>
-    <t>Growth_0.2_noMR_2</t>
-  </si>
-  <si>
     <t>Growth_0.8_MR_2</t>
   </si>
   <si>
-    <t>Growth_0.8_noMR_2</t>
-  </si>
-  <si>
     <t>Growth_3.2_MR_2</t>
   </si>
   <si>
-    <t>Growth_3.2_noMR_2</t>
-  </si>
-  <si>
     <t>Growth_0.4_MR_2</t>
   </si>
   <si>
-    <t>Growth_0.4_noMR_2</t>
-  </si>
-  <si>
     <t>Growth_0.1_MR_3</t>
   </si>
   <si>
-    <t>Growth_0.1_noMR_3</t>
-  </si>
-  <si>
     <t>Growth_0.2_MR_3</t>
   </si>
   <si>
-    <t>Growth_0.2_noMR_3</t>
-  </si>
-  <si>
     <t>Growth_0.8_MR_3</t>
   </si>
   <si>
-    <t>Growth_0.8_noMR_3</t>
-  </si>
-  <si>
     <t>Growth_3.2_MR_3</t>
   </si>
   <si>
-    <t>Growth_3.2_noMR_3</t>
-  </si>
-  <si>
     <t>Growth_0.4_MR_3</t>
   </si>
   <si>
-    <t>Growth_0.4_noMR_3</t>
-  </si>
-  <si>
     <t>Experiment</t>
   </si>
   <si>
@@ -140,111 +92,57 @@
     <t>Growth_1.6_MR_3</t>
   </si>
   <si>
-    <t>Growth_1.6_noMR_3</t>
-  </si>
-  <si>
-    <t>Growth_1.6_noMR_2</t>
-  </si>
-  <si>
     <t>Growth_1.6_MR_2</t>
   </si>
   <si>
     <t>Growth_0.1_MR_4</t>
   </si>
   <si>
-    <t>Growth_0.1_noMR_4</t>
-  </si>
-  <si>
     <t>Growth_0.2_MR_4</t>
   </si>
   <si>
-    <t>Growth_0.2_noMR_4</t>
-  </si>
-  <si>
     <t>Growth_0.8_MR_4</t>
   </si>
   <si>
-    <t>Growth_0.8_noMR_4</t>
-  </si>
-  <si>
     <t>Growth_1.6_MR_4</t>
   </si>
   <si>
-    <t>Growth_1.6_noMR_4</t>
-  </si>
-  <si>
     <t>Growth_3.2_MR_4</t>
   </si>
   <si>
-    <t>Growth_3.2_noMR_4</t>
-  </si>
-  <si>
     <t>Growth_0.4_MR_4</t>
   </si>
   <si>
-    <t>Growth_0.4_noMR_4</t>
-  </si>
-  <si>
     <t>Growth_0.1_MR_5</t>
   </si>
   <si>
-    <t>Growth_0.1_noMR_5</t>
-  </si>
-  <si>
     <t>Growth_0.2_MR_5</t>
   </si>
   <si>
-    <t>Growth_0.2_noMR_5</t>
-  </si>
-  <si>
     <t>Growth_0.8_MR_5</t>
   </si>
   <si>
-    <t>Growth_0.8_noMR_5</t>
-  </si>
-  <si>
     <t>Growth_1.6_MR_5</t>
   </si>
   <si>
-    <t>Growth_1.6_noMR_5</t>
-  </si>
-  <si>
     <t>Growth_3.2_MR_5</t>
   </si>
   <si>
-    <t>Growth_3.2_noMR_5</t>
-  </si>
-  <si>
     <t>Growth_0.4_MR_5</t>
   </si>
   <si>
-    <t>Growth_0.4_noMR_5</t>
-  </si>
-  <si>
     <t>Growth_0.1_MR_6</t>
   </si>
   <si>
-    <t>Growth_0.1_noMR_6</t>
-  </si>
-  <si>
     <t>Growth_0.2_MR_6</t>
   </si>
   <si>
-    <t>Growth_0.2_noMR_6</t>
-  </si>
-  <si>
     <t>Growth_0.1_MR_7</t>
   </si>
   <si>
-    <t>Growth_0.1_noMR_7</t>
-  </si>
-  <si>
     <t>Growth_0.2_MR_7</t>
   </si>
   <si>
-    <t>Growth_0.2_noMR_7</t>
-  </si>
-  <si>
     <t>g_min</t>
   </si>
   <si>
@@ -254,13 +152,115 @@
     <t>Growth_0.3_MR_1</t>
   </si>
   <si>
-    <t>Growth_0.3_noMR_1</t>
+    <t>Growth_0.1_NoMR_1</t>
+  </si>
+  <si>
+    <t>Growth_0.1_NoMR_2</t>
+  </si>
+  <si>
+    <t>Growth_0.1_NoMR_3</t>
+  </si>
+  <si>
+    <t>Growth_0.1_NoMR_4</t>
+  </si>
+  <si>
+    <t>Growth_0.1_NoMR_5</t>
+  </si>
+  <si>
+    <t>Growth_0.1_NoMR_6</t>
+  </si>
+  <si>
+    <t>Growth_0.1_NoMR_7</t>
+  </si>
+  <si>
+    <t>Growth_0.2_NoMR_1</t>
+  </si>
+  <si>
+    <t>Growth_0.2_NoMR_2</t>
+  </si>
+  <si>
+    <t>Growth_0.2_NoMR_3</t>
+  </si>
+  <si>
+    <t>Growth_0.2_NoMR_4</t>
+  </si>
+  <si>
+    <t>Growth_0.2_NoMR_5</t>
+  </si>
+  <si>
+    <t>Growth_0.2_NoMR_6</t>
+  </si>
+  <si>
+    <t>Growth_0.2_NoMR_7</t>
+  </si>
+  <si>
+    <t>Growth_0.4_NoMR_1</t>
+  </si>
+  <si>
+    <t>Growth_0.4_NoMR_2</t>
+  </si>
+  <si>
+    <t>Growth_0.4_NoMR_3</t>
+  </si>
+  <si>
+    <t>Growth_0.4_NoMR_4</t>
+  </si>
+  <si>
+    <t>Growth_0.4_NoMR_5</t>
+  </si>
+  <si>
+    <t>Growth_0.8_NoMR_1</t>
+  </si>
+  <si>
+    <t>Growth_0.8_NoMR_2</t>
+  </si>
+  <si>
+    <t>Growth_0.8_NoMR_3</t>
+  </si>
+  <si>
+    <t>Growth_0.8_NoMR_4</t>
+  </si>
+  <si>
+    <t>Growth_0.8_NoMR_5</t>
+  </si>
+  <si>
+    <t>Growth_1.6_NoMR_1</t>
+  </si>
+  <si>
+    <t>Growth_1.6_NoMR_2</t>
+  </si>
+  <si>
+    <t>Growth_1.6_NoMR_3</t>
+  </si>
+  <si>
+    <t>Growth_1.6_NoMR_4</t>
+  </si>
+  <si>
+    <t>Growth_1.6_NoMR_5</t>
+  </si>
+  <si>
+    <t>Growth_3.2_NoMR_1</t>
+  </si>
+  <si>
+    <t>Growth_3.2_NoMR_2</t>
+  </si>
+  <si>
+    <t>Growth_3.2_NoMR_3</t>
+  </si>
+  <si>
+    <t>Growth_3.2_NoMR_4</t>
+  </si>
+  <si>
+    <t>Growth_3.2_NoMR_5</t>
+  </si>
+  <si>
+    <t>Growth_0.3_NoMR_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -652,45 +652,45 @@
   <dimension ref="A1:F71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C73" sqref="C73:C74"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1">
         <v>0.1</v>
@@ -705,12 +705,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1">
         <v>0.1</v>
@@ -725,12 +725,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C4" s="1">
         <v>0.1</v>
@@ -745,12 +745,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1">
         <v>0.1</v>
@@ -765,12 +765,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C6" s="1">
         <v>0.1</v>
@@ -785,12 +785,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C7" s="1">
         <v>0.1</v>
@@ -805,12 +805,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1">
         <v>0.1</v>
@@ -825,9 +825,9 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -845,12 +845,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C10" s="1">
         <v>0.1</v>
@@ -865,12 +865,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
         <v>0.1</v>
@@ -885,12 +885,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1">
         <v>0.1</v>
@@ -905,12 +905,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="C13" s="1">
         <v>0.1</v>
@@ -925,12 +925,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1">
         <v>0.1</v>
@@ -945,12 +945,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="C15" s="1">
         <v>0.1</v>
@@ -965,12 +965,12 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="C16" s="1">
         <v>0.2</v>
@@ -985,12 +985,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="C17" s="1">
         <v>0.2</v>
@@ -1005,12 +1005,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="C18" s="1">
         <v>0.2</v>
@@ -1025,12 +1025,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C19" s="1">
         <v>0.2</v>
@@ -1045,12 +1045,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C20" s="1">
         <v>0.2</v>
@@ -1065,12 +1065,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C21" s="1">
         <v>0.2</v>
@@ -1085,12 +1085,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1">
         <v>0.2</v>
@@ -1105,12 +1105,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1">
         <v>0.2</v>
@@ -1125,12 +1125,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1">
         <v>0.2</v>
@@ -1145,12 +1145,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C25" s="1">
         <v>0.2</v>
@@ -1165,12 +1165,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C26" s="1">
         <v>0.2</v>
@@ -1185,12 +1185,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="C27" s="1">
         <v>0.2</v>
@@ -1205,12 +1205,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
         <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>67</v>
       </c>
       <c r="C28" s="1">
         <v>0.2</v>
@@ -1225,12 +1225,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="C29" s="1">
         <v>0.2</v>
@@ -1245,12 +1245,12 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="C30" s="1">
         <v>0.4</v>
@@ -1265,12 +1265,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="C31" s="1">
         <v>0.4</v>
@@ -1285,12 +1285,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C32" s="1">
         <v>0.4</v>
@@ -1305,12 +1305,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C33" s="1">
         <v>0.4</v>
@@ -1325,12 +1325,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1">
         <v>0.4</v>
@@ -1345,12 +1345,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C35" s="1">
         <v>0.4</v>
@@ -1365,12 +1365,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C36" s="1">
         <v>0.4</v>
@@ -1385,12 +1385,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C37" s="1">
         <v>0.4</v>
@@ -1405,12 +1405,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="C38" s="1">
         <v>0.4</v>
@@ -1425,12 +1425,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="C39" s="1">
         <v>0.4</v>
@@ -1445,12 +1445,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C40" s="1">
         <v>0.8</v>
@@ -1465,12 +1465,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1">
         <v>0.8</v>
@@ -1485,12 +1485,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C42" s="1">
         <v>0.8</v>
@@ -1505,12 +1505,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C43" s="1">
         <v>0.8</v>
@@ -1525,12 +1525,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C44" s="1">
         <v>0.8</v>
@@ -1545,12 +1545,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C45" s="1">
         <v>0.8</v>
@@ -1565,12 +1565,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C46" s="1">
         <v>0.8</v>
@@ -1585,12 +1585,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C47" s="1">
         <v>0.8</v>
@@ -1605,12 +1605,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="C48" s="1">
         <v>0.8</v>
@@ -1625,12 +1625,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C49" s="1">
         <v>0.8</v>
@@ -1645,12 +1645,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C50" s="1">
         <v>1.6</v>
@@ -1665,12 +1665,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="C51" s="1">
         <v>1.6</v>
@@ -1685,12 +1685,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C52" s="1">
         <v>1.6</v>
@@ -1705,12 +1705,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="C53" s="1">
         <v>1.6</v>
@@ -1725,12 +1725,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C54" s="1">
         <v>1.6</v>
@@ -1745,12 +1745,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C55" s="1">
         <v>1.6</v>
@@ -1765,12 +1765,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C56" s="1">
         <v>1.6</v>
@@ -1785,12 +1785,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C57" s="1">
         <v>1.6</v>
@@ -1805,12 +1805,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="C58" s="1">
         <v>1.6</v>
@@ -1825,12 +1825,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C59" s="1">
         <v>1.6</v>
@@ -1845,12 +1845,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="C60" s="1">
         <v>3.2</v>
@@ -1865,12 +1865,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B61" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C61" s="1">
         <v>3.2</v>
@@ -1885,12 +1885,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="C62" s="1">
         <v>3.2</v>
@@ -1905,12 +1905,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="C63" s="1">
         <v>3.2</v>
@@ -1925,12 +1925,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C64" s="1">
         <v>3.2</v>
@@ -1945,12 +1945,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C65" s="1">
         <v>3.2</v>
@@ -1965,12 +1965,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B66" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C66" s="1">
         <v>3.2</v>
@@ -1985,12 +1985,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C67" s="1">
         <v>3.2</v>
@@ -2005,12 +2005,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C68" s="1">
         <v>3.2</v>
@@ -2025,12 +2025,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B69" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="C69" s="1">
         <v>3.2</v>
@@ -2045,12 +2045,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C70" s="1">
         <v>0.3</v>
@@ -2065,9 +2065,9 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B71" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
Data analyzed through all the way
</commit_message>
<xml_diff>
--- a/DataIndex.xlsx
+++ b/DataIndex.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel\AppData\Local\Temp\scp00500\afs\crc.nd.edu\group\Zartman\Pavel\Project3Episcale\Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pavel\AppData\Local\Temp\scp14179\afs\crc.nd.edu\group\Zartman\Pavel\Project3Episcale\Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="84">
   <si>
     <t>Growth_0.1_MR_1</t>
   </si>
@@ -255,6 +255,27 @@
   </si>
   <si>
     <t>Growth_0.3_NoMR_1</t>
+  </si>
+  <si>
+    <t>Growth_0.3_MR_2</t>
+  </si>
+  <si>
+    <t>Growth_0.3_MR_3</t>
+  </si>
+  <si>
+    <t>Growth_0.3_MR_4</t>
+  </si>
+  <si>
+    <t>Growth_0.3_MR_5</t>
+  </si>
+  <si>
+    <t>Growth_0.3_NoMR_2</t>
+  </si>
+  <si>
+    <t>Growth_0.3_NoMR_3</t>
+  </si>
+  <si>
+    <t>Growth_0.3_NoMR_4</t>
   </si>
 </sst>
 </file>
@@ -649,11 +670,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F71"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,19 +1271,19 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="C30" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D30" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>0.3</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="F30" s="1">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1270,19 +1291,19 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="C31" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>0.3</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="F31" s="1">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1290,19 +1311,19 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C32" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D32" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <v>0.3</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="F32" s="1">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1310,19 +1331,19 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="C33" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D33" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>0.3</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="F33" s="1">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -1330,19 +1351,19 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="C34" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D34" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="1">
-        <v>0.3</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="F34" s="1">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -1350,19 +1371,19 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="C35" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D35" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E35" s="1">
-        <v>0.3</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="F35" s="1">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -1370,19 +1391,19 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="C36" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D36" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E36" s="1">
-        <v>0.3</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="F36" s="1">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1390,19 +1411,19 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>79</v>
       </c>
       <c r="C37" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D37" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E37" s="1">
-        <v>0.3</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="F37" s="1">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1410,19 +1431,19 @@
         <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="C38" s="1">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D38" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E38" s="1">
-        <v>0.3</v>
+        <v>0.22499999999999998</v>
       </c>
       <c r="F38" s="1">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1430,13 +1451,13 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C39" s="1">
         <v>0.4</v>
       </c>
       <c r="D39" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1">
         <v>0.3</v>
@@ -1450,19 +1471,19 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C40" s="1">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D40" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E40" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F40" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1470,19 +1491,19 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C41" s="1">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D41" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F41" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1490,19 +1511,19 @@
         <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C42" s="1">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D42" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F42" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1510,19 +1531,19 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C43" s="1">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D43" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E43" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F43" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1530,19 +1551,19 @@
         <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="C44" s="1">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D44" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F44" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1550,19 +1571,19 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="C45" s="1">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D45" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E45" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F45" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1570,19 +1591,19 @@
         <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C46" s="1">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D46" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E46" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F46" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1590,19 +1611,19 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C47" s="1">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D47" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E47" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F47" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1610,19 +1631,19 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C48" s="1">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="D48" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E48" s="1">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="F48" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1630,13 +1651,13 @@
         <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C49" s="1">
         <v>0.8</v>
       </c>
       <c r="D49" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49" s="1">
         <v>0.6</v>
@@ -1650,19 +1671,19 @@
         <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C50" s="1">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="D50" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E50" s="1">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F50" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1670,19 +1691,19 @@
         <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C51" s="1">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="D51" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E51" s="1">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F51" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1690,19 +1711,19 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C52" s="1">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="D52" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E52" s="1">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F52" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1710,19 +1731,19 @@
         <v>20</v>
       </c>
       <c r="B53" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C53" s="1">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="D53" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E53" s="1">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F53" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1730,19 +1751,19 @@
         <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="C54" s="1">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="D54" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54" s="1">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F54" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1750,19 +1771,19 @@
         <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C55" s="1">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="D55" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E55" s="1">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F55" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1770,19 +1791,19 @@
         <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C56" s="1">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="D56" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E56" s="1">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F56" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1790,19 +1811,19 @@
         <v>20</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C57" s="1">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="D57" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E57" s="1">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F57" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1810,19 +1831,19 @@
         <v>20</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C58" s="1">
-        <v>1.6</v>
+        <v>0.8</v>
       </c>
       <c r="D58" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E58" s="1">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="F58" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1830,13 +1851,13 @@
         <v>20</v>
       </c>
       <c r="B59" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C59" s="1">
         <v>1.6</v>
       </c>
       <c r="D59" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59" s="1">
         <v>1.2</v>
@@ -1850,19 +1871,19 @@
         <v>20</v>
       </c>
       <c r="B60" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C60" s="1">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="D60" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E60" s="1">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="F60" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1870,19 +1891,19 @@
         <v>20</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C61" s="1">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="D61" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E61" s="1">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="F61" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1890,19 +1911,19 @@
         <v>20</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C62" s="1">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="D62" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E62" s="1">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="F62" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1910,19 +1931,19 @@
         <v>20</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C63" s="1">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="D63" s="1" t="b">
         <v>0</v>
       </c>
       <c r="E63" s="1">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="F63" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1930,19 +1951,19 @@
         <v>20</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="C64" s="1">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="D64" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64" s="1">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="F64" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1950,19 +1971,19 @@
         <v>20</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C65" s="1">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="D65" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E65" s="1">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="F65" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1970,19 +1991,19 @@
         <v>20</v>
       </c>
       <c r="B66" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C66" s="1">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="D66" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E66" s="1">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="F66" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1990,19 +2011,19 @@
         <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C67" s="1">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="D67" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E67" s="1">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="F67" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -2010,19 +2031,19 @@
         <v>20</v>
       </c>
       <c r="B68" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C68" s="1">
-        <v>3.2</v>
+        <v>1.6</v>
       </c>
       <c r="D68" s="1" t="b">
         <v>1</v>
       </c>
       <c r="E68" s="1">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
       <c r="F68" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2030,13 +2051,13 @@
         <v>20</v>
       </c>
       <c r="B69" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="C69" s="1">
         <v>3.2</v>
       </c>
       <c r="D69" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69" s="1">
         <v>2.4</v>
@@ -2050,19 +2071,19 @@
         <v>20</v>
       </c>
       <c r="B70" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="C70" s="1">
-        <v>0.3</v>
+        <v>3.2</v>
       </c>
       <c r="D70" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70" s="1">
-        <v>0.22499999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="F70" s="1">
-        <v>0.375</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2070,25 +2091,165 @@
         <v>20</v>
       </c>
       <c r="B71" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C71" s="1">
-        <v>0.3</v>
+        <v>3.2</v>
       </c>
       <c r="D71" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71" s="1">
-        <v>0.22499999999999998</v>
+        <v>2.4</v>
       </c>
       <c r="F71" s="1">
-        <v>0.375</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D72" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F72" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" t="s">
+        <v>75</v>
+      </c>
+      <c r="C73" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D73" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F73" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D74" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E74" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F74" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" t="s">
+        <v>12</v>
+      </c>
+      <c r="C75" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D75" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E75" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F75" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>20</v>
+      </c>
+      <c r="B76" t="s">
+        <v>17</v>
+      </c>
+      <c r="C76" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D76" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F76" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" t="s">
+        <v>27</v>
+      </c>
+      <c r="C77" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D77" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E77" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F77" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" t="s">
+        <v>33</v>
+      </c>
+      <c r="C78" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="D78" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E78" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="F78" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D80">
-    <sortCondition ref="C2:C80"/>
-    <sortCondition ref="D2:D80"/>
+  <sortState ref="A2:F78">
+    <sortCondition ref="C2:C78"/>
+    <sortCondition ref="D2:D78"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>